<commit_message>
Revamp AVLExternalJob test. Bugs corrected in analysis file reading functions. TODO: check statements with if(varName.function() || varName == null) - swap the order of tests to avoid NullPointerException
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72_AVL/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72_AVL/BALANCE/Balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="48">
   <si>
     <t>Description</t>
   </si>
@@ -43,6 +43,9 @@
     <t>m</t>
   </si>
   <si>
+    <t>Zcg structure MAC</t>
+  </si>
+  <si>
     <t>Zcg structure BRF</t>
   </si>
   <si>
@@ -55,6 +58,9 @@
     <t>Xcg structure and engines BRF</t>
   </si>
   <si>
+    <t>Zcg structure and engines MAC</t>
+  </si>
+  <si>
     <t>Zcg structure and engines BRF</t>
   </si>
   <si>
@@ -64,6 +70,9 @@
     <t>Xcg operating empty mass BRF</t>
   </si>
   <si>
+    <t>Zcg operating empty mass MAC</t>
+  </si>
+  <si>
     <t>Zcg operating empty mass BRF</t>
   </si>
   <si>
@@ -73,6 +82,9 @@
     <t>Xcg maximum zero fuel mass BRF</t>
   </si>
   <si>
+    <t>Zcg maximum zero fuel mass MAC</t>
+  </si>
+  <si>
     <t>Zcg maximum zero fuel mass BRF</t>
   </si>
   <si>
@@ -82,7 +94,16 @@
     <t>Xcg maximum take-off mass BRF</t>
   </si>
   <si>
+    <t>Zcg maximum take-off mass MAC</t>
+  </si>
+  <si>
     <t>Zcg maximum take-off mass BRF</t>
+  </si>
+  <si>
+    <t>Max forward Xcg MAC</t>
+  </si>
+  <si>
+    <t>Max aft Xcg MAC</t>
   </si>
   <si>
     <t>Xcg LRF</t>
@@ -209,6 +230,10 @@
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <cols>
+    <col min="2" max="2" width="8.0" customWidth="true"/>
+    <col min="3" max="3" width="15.0" customWidth="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -229,7 +254,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>5.236520021021633</v>
+        <v>59.713422376876515</v>
       </c>
     </row>
     <row r="3">
@@ -240,7 +265,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>12.240997717128838</v>
+        <v>12.559202753573263</v>
       </c>
     </row>
     <row r="4">
@@ -248,26 +273,26 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6576665053638682</v>
+        <v>24.183035275777005</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.5567940147707489</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="n">
-        <v>5.041226939529571</v>
       </c>
     </row>
     <row r="7">
@@ -275,10 +300,10 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>11.791351849019662</v>
+        <v>37.64967967534197</v>
       </c>
     </row>
     <row r="8">
@@ -289,34 +314,34 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.721704678058392</v>
+        <v>12.051203664974096</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="n">
+        <v>27.7443608580375</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>5.041226939529571</v>
+        <v>0.6387905361436799</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="n">
-        <v>11.791351849019662</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
@@ -324,91 +349,168 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C12" t="n">
-        <v>0.721704678058392</v>
+        <v>37.64967967534197</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="n">
+        <v>12.051203664974096</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>5.081355335965858</v>
+        <v>27.7443608580375</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>11.883744101287732</v>
+        <v>0.6387905361436799</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.46534746772689106</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="n">
+        <v>38.11006187231468</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C18" t="n">
-        <v>4.974961100839947</v>
+        <v>12.061803577220768</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C19" t="n">
-        <v>11.638780337853301</v>
+        <v>17.71402417054916</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>0.6736251083832776</v>
+        <v>0.4078504837457484</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="n">
+        <v>38.17000310854741</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="n">
+        <v>12.063183673688883</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" t="n">
+        <v>24.874486492604568</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.5727140965406816</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="n">
+        <v>22.567166577937645</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="n">
+        <v>53.01505405947178</v>
       </c>
     </row>
   </sheetData>
@@ -422,7 +524,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="25"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <cols>
+    <col min="2" max="2" width="8.0" customWidth="true"/>
+    <col min="3" max="3" width="15.0" customWidth="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -437,18 +543,18 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>10.669199572303402</v>
+        <v>11.04753745546374</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -459,7 +565,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -470,23 +576,23 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>10.669199572303402</v>
+        <v>11.04753745546374</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -497,7 +603,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -508,28 +614,28 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>10.74365914460681</v>
+        <v>11.500334910927485</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -549,7 +655,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="25"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <cols>
+    <col min="2" max="2" width="8.0" customWidth="true"/>
+    <col min="3" max="3" width="15.0" customWidth="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -564,18 +674,18 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>1.216893150576782</v>
+        <v>1.330689739372911</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -586,7 +696,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -597,23 +707,23 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>12.21689315057678</v>
+        <v>12.33068973937291</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -624,7 +734,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -635,65 +745,43 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.13133814372353347</v>
+        <v>1.330689739372911</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1.216893150576782</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="n">
-        <v>20.71853476770793</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="n">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="n">
         <v>4.735499999999998</v>
       </c>
     </row>
@@ -708,7 +796,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="25"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <cols>
+    <col min="2" max="2" width="8.0" customWidth="true"/>
+    <col min="3" max="3" width="15.0" customWidth="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -723,18 +815,18 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>1.0771659522222063</v>
+        <v>1.0717832283332958</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -745,7 +837,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -756,23 +848,23 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>12.077165952222204</v>
+        <v>12.071783228333294</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -783,7 +875,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -794,7 +886,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -808,7 +900,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="25"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <cols>
+    <col min="2" max="2" width="8.0" customWidth="true"/>
+    <col min="3" max="3" width="15.0" customWidth="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -823,18 +919,18 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6614514340216029</v>
+        <v>0.8841681842937887</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -845,7 +941,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -856,23 +952,23 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>25.9614514340216</v>
+        <v>26.184168184293785</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -883,7 +979,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -894,38 +990,38 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>0.6614514340216029</v>
+        <v>0.8841681842937887</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -945,7 +1041,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="25"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <cols>
+    <col min="2" max="2" width="8.0" customWidth="true"/>
+    <col min="3" max="3" width="15.0" customWidth="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -960,18 +1060,18 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>2.5640710746536346</v>
+        <v>2.5640710746536337</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -982,7 +1082,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -993,12 +1093,12 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1009,7 +1109,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1020,49 +1120,49 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>1.8315999999999997</v>
+        <v>3.1315999999999997</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>2.5640710746536346</v>
+        <v>2.5640710746536337</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -1082,7 +1182,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="25"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <cols>
+    <col min="2" max="2" width="8.0" customWidth="true"/>
+    <col min="3" max="3" width="15.0" customWidth="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -1097,22 +1201,22 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -1123,7 +1227,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1134,7 +1238,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1145,12 +1249,12 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -1161,7 +1265,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -1172,7 +1276,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1183,27 +1287,27 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -1214,7 +1318,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -1225,7 +1329,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -1236,12 +1340,12 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -1252,7 +1356,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -1263,7 +1367,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -1274,17 +1378,17 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1298,7 +1402,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="25"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <cols>
+    <col min="2" max="2" width="8.0" customWidth="true"/>
+    <col min="3" max="3" width="15.0" customWidth="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -1313,22 +1421,22 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -1339,7 +1447,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1350,7 +1458,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1361,12 +1469,12 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -1377,7 +1485,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -1388,7 +1496,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1399,27 +1507,27 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -1430,7 +1538,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -1441,7 +1549,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -1452,12 +1560,12 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -1468,7 +1576,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -1479,7 +1587,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -1490,17 +1598,17 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1514,7 +1622,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="25"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <cols>
+    <col min="2" max="2" width="8.0" customWidth="true"/>
+    <col min="3" max="3" width="15.0" customWidth="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -1529,18 +1641,18 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>12.299024241711926</v>
+        <v>12.183956107332701</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1551,18 +1663,18 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.674638699878493</v>
+        <v>-1.8746386998784927</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>